<commit_message>
it now reads/writes to same file
Now the code will read and write to the same file. It will write the TA
to a different tab and re-save the file in the end, provided you change
the area it grabs from the time series tab (sheet 1) and change the tab
it writes things back with on line 115.

Next, I'll try to just have it read all the data and output it all to
the same tab. Baby steps, though.
</commit_message>
<xml_diff>
--- a/anakyzed.xlsx
+++ b/anakyzed.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -509,13 +510,13 @@
   </sheetPr>
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.69140625" defaultRowHeight="14.6" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="16384" min="1" style="2" width="8.7265625"/>
+    <col customWidth="1" max="16384" min="1" style="2" width="8.69140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -1739,103 +1740,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.69140625" defaultRowHeight="14.6" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="16384" min="1" style="2" width="8.7265625"/>
+    <col customWidth="1" max="16384" min="1" style="2" width="8.69140625"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="n">
-        <v>432.9604174527465</v>
-      </c>
-      <c r="B1" t="n">
-        <v>157.6565028933628</v>
-      </c>
-      <c r="C1" t="n">
-        <v>100.5364509608477</v>
-      </c>
-      <c r="D1" t="n">
-        <v>18227.31949667334</v>
-      </c>
-      <c r="E1" t="n">
-        <v>32333.18085156193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="n">
-        <v>385.142419893523</v>
-      </c>
-      <c r="B2" t="n">
-        <v>129.2841508036708</v>
-      </c>
-      <c r="C2" t="n">
-        <v>108.1996807442682</v>
-      </c>
-      <c r="D2" t="n">
-        <v>15114.84829987815</v>
-      </c>
-      <c r="E2" t="n">
-        <v>27581.36118929135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="n">
-        <v>394.386171867544</v>
-      </c>
-      <c r="B3" t="n">
-        <v>112.375937966617</v>
-      </c>
-      <c r="C3" t="n">
-        <v>99.18737151716449</v>
-      </c>
-      <c r="D3" t="n">
-        <v>18998.32671603235</v>
-      </c>
-      <c r="E3" t="n">
-        <v>34296.39049633301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="n">
-        <v>360.5405392709662</v>
-      </c>
-      <c r="B4" t="n">
-        <v>143.7304524680481</v>
-      </c>
-      <c r="C4" t="n">
-        <v>96.09587923489934</v>
-      </c>
-      <c r="D4" t="n">
-        <v>14776.90709735898</v>
-      </c>
-      <c r="E4" t="n">
-        <v>24512.81392866398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="n">
-        <v>393.2573871211949</v>
-      </c>
-      <c r="B5" t="n">
-        <v>136.1244179741812</v>
-      </c>
-      <c r="C5" t="n">
-        <v>101.9325706731346</v>
-      </c>
-      <c r="D5" t="n">
-        <v>16779.35040248571</v>
-      </c>
-      <c r="E5" t="n">
-        <v>29680.93661646252</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.5118055555555555" header="0.5118055555555555" left="0.7" right="0.7" top="0.75"/>
   <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
@@ -1847,18 +1762,88 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.69140625" defaultRowHeight="14.6" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="16384" min="1" style="2" width="8.7265625"/>
+    <col customWidth="1" max="16384" min="1" style="2" width="8.69140625"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="n">
+        <v>432.9604174527465</v>
+      </c>
+      <c r="B1" t="n">
+        <v>157.6565028933628</v>
+      </c>
+      <c r="C1" t="n">
+        <v>100.5364509608477</v>
+      </c>
+      <c r="D1" t="n">
+        <v>19069.94516042675</v>
+      </c>
+      <c r="E1" t="n">
+        <v>31490.55518780852</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="n">
+        <v>385.142419893523</v>
+      </c>
+      <c r="B2" t="n">
+        <v>129.2841508036708</v>
+      </c>
+      <c r="C2" t="n">
+        <v>108.1996807442682</v>
+      </c>
+      <c r="D2" t="n">
+        <v>15891.04308403571</v>
+      </c>
+      <c r="E2" t="n">
+        <v>26805.16640513378</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="n">
+        <v>409.0514186731344</v>
+      </c>
+      <c r="B3" t="n">
+        <v>143.7454045971708</v>
+      </c>
+      <c r="C3" t="n">
+        <v>104.9459852064982</v>
+      </c>
+      <c r="D3" t="n">
+        <v>17480.49412223122</v>
+      </c>
+      <c r="E3" t="n">
+        <v>29147.8607964711</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="0.75" footer="0.5118055555555555" header="0.5118055555555555" left="0.7" right="0.7" top="0.75"/>
   <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.45"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>